<commit_message>
[V0.0.0] Page transaction (ajout Tableau)
</commit_message>
<xml_diff>
--- a/Documentation/maquette.xlsx
+++ b/Documentation/maquette.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20367"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\XS2E1356\Desktop\Autres\perso\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\budgetiz\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4ED4CE6-74AF-453E-942B-E4FA77066C4E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE8DC4A2-070C-47A6-AB72-27A8BF1ACE69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8100" tabRatio="857" activeTab="5" xr2:uid="{C2AFE70A-D351-4C3B-BEED-FD22DDFED1E9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="857" activeTab="5" xr2:uid="{C2AFE70A-D351-4C3B-BEED-FD22DDFED1E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="9" r:id="rId1"/>
@@ -45,6 +45,13 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -2851,178 +2858,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
@@ -3046,29 +2912,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -3086,6 +2931,168 @@
     <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Insatisfaisant" xfId="4" builtinId="27"/>
@@ -5194,7 +5201,7 @@
         <xdr:cNvPr id="3" name="Graphique 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0C00-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5230,7 +5237,7 @@
         <xdr:cNvPr id="4" name="Graphique 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0C00-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5276,7 +5283,7 @@
                   <a14:compatExt spid="_x0000_s4101"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005100000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0D00-000005100000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5343,7 +5350,7 @@
                   <a14:compatExt spid="_x0000_s4104"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008100000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0D00-000008100000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5410,7 +5417,7 @@
                   <a14:compatExt spid="_x0000_s4105"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000009100000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0D00-000009100000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5477,7 +5484,7 @@
                   <a14:compatExt spid="_x0000_s4106"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000A100000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0D00-00000A100000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5544,7 +5551,7 @@
                   <a14:compatExt spid="_x0000_s4110"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00000E100000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0D00-00000E100000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5611,7 +5618,7 @@
                   <a14:compatExt spid="_x0000_s4113"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B99426EE-B814-4A19-A5E3-413182CA0A99}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0D00-000011100000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -6024,28 +6031,28 @@
   </cols>
   <sheetData>
     <row r="15" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E15" s="84" t="s">
+      <c r="E15" s="123" t="s">
         <v>120</v>
       </c>
-      <c r="F15" s="85"/>
-      <c r="G15" s="100" t="s">
+      <c r="F15" s="125"/>
+      <c r="G15" s="119" t="s">
         <v>119</v>
       </c>
-      <c r="H15" s="101"/>
-      <c r="I15" s="102"/>
-      <c r="J15" s="89" t="s">
+      <c r="H15" s="130"/>
+      <c r="I15" s="120"/>
+      <c r="J15" s="124" t="s">
         <v>121</v>
       </c>
-      <c r="K15" s="85"/>
+      <c r="K15" s="125"/>
     </row>
     <row r="16" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E16" s="86"/>
-      <c r="F16" s="87"/>
-      <c r="G16" s="103"/>
-      <c r="H16" s="104"/>
-      <c r="I16" s="105"/>
-      <c r="J16" s="90"/>
-      <c r="K16" s="87"/>
+      <c r="E16" s="126"/>
+      <c r="F16" s="128"/>
+      <c r="G16" s="121"/>
+      <c r="H16" s="131"/>
+      <c r="I16" s="122"/>
+      <c r="J16" s="127"/>
+      <c r="K16" s="128"/>
     </row>
     <row r="17" spans="5:17" x14ac:dyDescent="0.25">
       <c r="G17" s="16"/>
@@ -6053,19 +6060,19 @@
       <c r="I17" s="16"/>
     </row>
     <row r="18" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E18" s="81" t="s">
+      <c r="E18" s="129" t="s">
         <v>122</v>
       </c>
-      <c r="F18" s="81"/>
+      <c r="F18" s="129"/>
     </row>
     <row r="20" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E20" s="82" t="s">
+      <c r="E20" s="72" t="s">
         <v>123</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="H20" s="83" t="s">
+      <c r="H20" s="73" t="s">
         <v>127</v>
       </c>
       <c r="J20" s="13" t="s">
@@ -6077,28 +6084,28 @@
       <c r="N20" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="P20" s="67" t="s">
+      <c r="P20" s="109" t="s">
         <v>129</v>
       </c>
-      <c r="Q20" s="67"/>
+      <c r="Q20" s="109"/>
     </row>
     <row r="24" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E24" s="114" t="s">
+      <c r="E24" s="79" t="s">
         <v>124</v>
       </c>
-      <c r="F24" s="93" t="s">
+      <c r="F24" s="114" t="s">
         <v>125</v>
       </c>
-      <c r="G24" s="96"/>
-      <c r="H24" s="91" t="s">
+      <c r="G24" s="115"/>
+      <c r="H24" s="116" t="s">
         <v>142</v>
       </c>
-      <c r="I24" s="91"/>
-      <c r="J24" s="91"/>
-      <c r="K24" s="98" t="s">
+      <c r="I24" s="116"/>
+      <c r="J24" s="116"/>
+      <c r="K24" s="75" t="s">
         <v>130</v>
       </c>
-      <c r="L24" s="92" t="s">
+      <c r="L24" s="74" t="s">
         <v>131</v>
       </c>
       <c r="N24" s="16"/>
@@ -6108,16 +6115,16 @@
       <c r="E25">
         <v>1</v>
       </c>
-      <c r="F25" s="94" t="s">
+      <c r="F25" s="117" t="s">
         <v>89</v>
       </c>
-      <c r="G25" s="97"/>
-      <c r="H25" s="68" t="s">
+      <c r="G25" s="118"/>
+      <c r="H25" s="108" t="s">
         <v>28</v>
       </c>
-      <c r="I25" s="68"/>
-      <c r="J25" s="68"/>
-      <c r="K25" s="99" t="s">
+      <c r="I25" s="108"/>
+      <c r="J25" s="108"/>
+      <c r="K25" s="76" t="s">
         <v>132</v>
       </c>
       <c r="L25" s="16" t="s">
@@ -6130,16 +6137,16 @@
       <c r="E26">
         <v>2</v>
       </c>
-      <c r="F26" s="94" t="s">
+      <c r="F26" s="117" t="s">
         <v>140</v>
       </c>
-      <c r="G26" s="97"/>
-      <c r="H26" s="68" t="s">
+      <c r="G26" s="118"/>
+      <c r="H26" s="108" t="s">
         <v>28</v>
       </c>
-      <c r="I26" s="68"/>
-      <c r="J26" s="68"/>
-      <c r="K26" s="99" t="s">
+      <c r="I26" s="108"/>
+      <c r="J26" s="108"/>
+      <c r="K26" s="76" t="s">
         <v>132</v>
       </c>
       <c r="L26" s="16" t="s">
@@ -6152,16 +6159,16 @@
       <c r="E27">
         <v>3</v>
       </c>
-      <c r="F27" s="94" t="s">
+      <c r="F27" s="117" t="s">
         <v>2</v>
       </c>
-      <c r="G27" s="97"/>
-      <c r="H27" s="68" t="s">
+      <c r="G27" s="118"/>
+      <c r="H27" s="108" t="s">
         <v>28</v>
       </c>
-      <c r="I27" s="68"/>
-      <c r="J27" s="68"/>
-      <c r="K27" s="99" t="s">
+      <c r="I27" s="108"/>
+      <c r="J27" s="108"/>
+      <c r="K27" s="76" t="s">
         <v>132</v>
       </c>
       <c r="L27" s="16" t="s">
@@ -6174,16 +6181,16 @@
       <c r="E28">
         <v>4</v>
       </c>
-      <c r="F28" s="94" t="s">
+      <c r="F28" s="117" t="s">
         <v>2</v>
       </c>
-      <c r="G28" s="97"/>
-      <c r="H28" s="68" t="s">
+      <c r="G28" s="118"/>
+      <c r="H28" s="108" t="s">
         <v>95</v>
       </c>
-      <c r="I28" s="68"/>
-      <c r="J28" s="68"/>
-      <c r="K28" s="99" t="s">
+      <c r="I28" s="108"/>
+      <c r="J28" s="108"/>
+      <c r="K28" s="76" t="s">
         <v>132</v>
       </c>
       <c r="L28" s="16" t="s">
@@ -6196,16 +6203,16 @@
       <c r="E29">
         <v>5</v>
       </c>
-      <c r="F29" s="94" t="s">
+      <c r="F29" s="117" t="s">
         <v>3</v>
       </c>
-      <c r="G29" s="97"/>
-      <c r="H29" s="68" t="s">
+      <c r="G29" s="118"/>
+      <c r="H29" s="108" t="s">
         <v>95</v>
       </c>
-      <c r="I29" s="68"/>
-      <c r="J29" s="68"/>
-      <c r="K29" s="99" t="s">
+      <c r="I29" s="108"/>
+      <c r="J29" s="108"/>
+      <c r="K29" s="76" t="s">
         <v>132</v>
       </c>
       <c r="L29" s="16" t="s">
@@ -6218,16 +6225,16 @@
       <c r="E30">
         <v>6</v>
       </c>
-      <c r="F30" s="94" t="s">
+      <c r="F30" s="117" t="s">
         <v>141</v>
       </c>
-      <c r="G30" s="97"/>
-      <c r="H30" s="68" t="s">
+      <c r="G30" s="118"/>
+      <c r="H30" s="108" t="s">
         <v>95</v>
       </c>
-      <c r="I30" s="68"/>
-      <c r="J30" s="68"/>
-      <c r="K30" s="99" t="s">
+      <c r="I30" s="108"/>
+      <c r="J30" s="108"/>
+      <c r="K30" s="76" t="s">
         <v>132</v>
       </c>
       <c r="L30" s="16" t="s">
@@ -6278,28 +6285,28 @@
   </cols>
   <sheetData>
     <row r="15" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E15" s="84" t="s">
+      <c r="E15" s="123" t="s">
         <v>120</v>
       </c>
-      <c r="F15" s="85"/>
-      <c r="G15" s="107" t="s">
+      <c r="F15" s="125"/>
+      <c r="G15" s="132" t="s">
         <v>119</v>
       </c>
-      <c r="H15" s="108"/>
-      <c r="I15" s="109"/>
-      <c r="J15" s="101" t="s">
+      <c r="H15" s="133"/>
+      <c r="I15" s="134"/>
+      <c r="J15" s="130" t="s">
         <v>121</v>
       </c>
-      <c r="K15" s="102"/>
+      <c r="K15" s="120"/>
     </row>
     <row r="16" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E16" s="86"/>
-      <c r="F16" s="87"/>
-      <c r="G16" s="110"/>
-      <c r="H16" s="111"/>
-      <c r="I16" s="112"/>
-      <c r="J16" s="104"/>
-      <c r="K16" s="105"/>
+      <c r="E16" s="126"/>
+      <c r="F16" s="128"/>
+      <c r="G16" s="135"/>
+      <c r="H16" s="136"/>
+      <c r="I16" s="137"/>
+      <c r="J16" s="131"/>
+      <c r="K16" s="122"/>
     </row>
     <row r="17" spans="5:17" x14ac:dyDescent="0.25">
       <c r="G17" s="16"/>
@@ -6307,19 +6314,19 @@
       <c r="I17" s="16"/>
     </row>
     <row r="18" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E18" s="81" t="s">
+      <c r="E18" s="129" t="s">
         <v>122</v>
       </c>
-      <c r="F18" s="81"/>
+      <c r="F18" s="129"/>
     </row>
     <row r="20" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E20" s="82" t="s">
+      <c r="E20" s="72" t="s">
         <v>123</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="H20" s="83" t="s">
+      <c r="H20" s="73" t="s">
         <v>127</v>
       </c>
       <c r="J20" s="13" t="s">
@@ -6331,28 +6338,28 @@
       <c r="N20" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="P20" s="67" t="s">
+      <c r="P20" s="109" t="s">
         <v>129</v>
       </c>
-      <c r="Q20" s="67"/>
+      <c r="Q20" s="109"/>
     </row>
     <row r="24" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E24" s="114" t="s">
+      <c r="E24" s="79" t="s">
         <v>124</v>
       </c>
-      <c r="F24" s="93" t="s">
+      <c r="F24" s="114" t="s">
         <v>125</v>
       </c>
-      <c r="G24" s="96"/>
-      <c r="H24" s="91" t="s">
+      <c r="G24" s="115"/>
+      <c r="H24" s="116" t="s">
         <v>126</v>
       </c>
-      <c r="I24" s="91"/>
-      <c r="J24" s="91"/>
-      <c r="K24" s="98" t="s">
+      <c r="I24" s="116"/>
+      <c r="J24" s="116"/>
+      <c r="K24" s="75" t="s">
         <v>130</v>
       </c>
-      <c r="L24" s="92" t="s">
+      <c r="L24" s="74" t="s">
         <v>131</v>
       </c>
       <c r="N24" s="16"/>
@@ -6362,16 +6369,16 @@
       <c r="E25">
         <v>1</v>
       </c>
-      <c r="F25" s="94" t="s">
+      <c r="F25" s="117" t="s">
         <v>147</v>
       </c>
-      <c r="G25" s="97"/>
-      <c r="H25" s="68" t="s">
+      <c r="G25" s="118"/>
+      <c r="H25" s="108" t="s">
         <v>146</v>
       </c>
-      <c r="I25" s="68"/>
-      <c r="J25" s="68"/>
-      <c r="K25" s="99" t="s">
+      <c r="I25" s="108"/>
+      <c r="J25" s="108"/>
+      <c r="K25" s="76" t="s">
         <v>132</v>
       </c>
       <c r="L25" s="16" t="s">
@@ -6384,16 +6391,16 @@
       <c r="E26">
         <v>2</v>
       </c>
-      <c r="F26" s="94" t="s">
+      <c r="F26" s="117" t="s">
         <v>107</v>
       </c>
-      <c r="G26" s="97"/>
-      <c r="H26" s="68" t="s">
+      <c r="G26" s="118"/>
+      <c r="H26" s="108" t="s">
         <v>46</v>
       </c>
-      <c r="I26" s="68"/>
-      <c r="J26" s="68"/>
-      <c r="K26" s="99" t="s">
+      <c r="I26" s="108"/>
+      <c r="J26" s="108"/>
+      <c r="K26" s="76" t="s">
         <v>132</v>
       </c>
       <c r="L26" s="16" t="s">
@@ -6406,16 +6413,16 @@
       <c r="E27">
         <v>3</v>
       </c>
-      <c r="F27" s="94" t="s">
+      <c r="F27" s="117" t="s">
         <v>108</v>
       </c>
-      <c r="G27" s="97"/>
-      <c r="H27" s="68" t="s">
+      <c r="G27" s="118"/>
+      <c r="H27" s="108" t="s">
         <v>46</v>
       </c>
-      <c r="I27" s="68"/>
-      <c r="J27" s="68"/>
-      <c r="K27" s="99" t="s">
+      <c r="I27" s="108"/>
+      <c r="J27" s="108"/>
+      <c r="K27" s="76" t="s">
         <v>132</v>
       </c>
       <c r="L27" s="16" t="s">
@@ -6428,16 +6435,16 @@
       <c r="E28">
         <v>4</v>
       </c>
-      <c r="F28" s="94" t="s">
+      <c r="F28" s="117" t="s">
         <v>109</v>
       </c>
-      <c r="G28" s="97"/>
-      <c r="H28" s="68" t="s">
+      <c r="G28" s="118"/>
+      <c r="H28" s="108" t="s">
         <v>46</v>
       </c>
-      <c r="I28" s="68"/>
-      <c r="J28" s="68"/>
-      <c r="K28" s="99" t="s">
+      <c r="I28" s="108"/>
+      <c r="J28" s="108"/>
+      <c r="K28" s="76" t="s">
         <v>132</v>
       </c>
       <c r="L28" s="16" t="s">
@@ -6447,48 +6454,48 @@
       <c r="N28" s="16"/>
     </row>
     <row r="29" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="F29" s="94"/>
-      <c r="G29" s="97"/>
-      <c r="H29" s="68"/>
-      <c r="I29" s="68"/>
-      <c r="J29" s="68"/>
-      <c r="K29" s="99"/>
+      <c r="F29" s="117"/>
+      <c r="G29" s="118"/>
+      <c r="H29" s="108"/>
+      <c r="I29" s="108"/>
+      <c r="J29" s="108"/>
+      <c r="K29" s="76"/>
       <c r="L29" s="16"/>
       <c r="M29" s="16"/>
       <c r="N29" s="16"/>
     </row>
     <row r="30" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="F30" s="94"/>
-      <c r="G30" s="97"/>
-      <c r="H30" s="68"/>
-      <c r="I30" s="68"/>
-      <c r="J30" s="68"/>
-      <c r="K30" s="99"/>
+      <c r="F30" s="117"/>
+      <c r="G30" s="118"/>
+      <c r="H30" s="108"/>
+      <c r="I30" s="108"/>
+      <c r="J30" s="108"/>
+      <c r="K30" s="76"/>
       <c r="L30" s="16"/>
       <c r="M30" s="16"/>
       <c r="N30" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="H30:J30"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="H27:J27"/>
     <mergeCell ref="F28:G28"/>
     <mergeCell ref="H28:J28"/>
     <mergeCell ref="F29:G29"/>
     <mergeCell ref="H29:J29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="H30:J30"/>
+    <mergeCell ref="P20:Q20"/>
     <mergeCell ref="F25:G25"/>
     <mergeCell ref="H25:J25"/>
     <mergeCell ref="F26:G26"/>
     <mergeCell ref="H26:J26"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="H27:J27"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="H24:J24"/>
     <mergeCell ref="E15:F16"/>
     <mergeCell ref="G15:I16"/>
     <mergeCell ref="J15:K16"/>
     <mergeCell ref="E18:F18"/>
-    <mergeCell ref="P20:Q20"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="H24:J24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -6512,24 +6519,24 @@
   </cols>
   <sheetData>
     <row r="15" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E15" s="117" t="s">
+      <c r="E15" s="140" t="s">
         <v>171</v>
       </c>
-      <c r="F15" s="117"/>
-      <c r="G15" s="116"/>
-      <c r="H15" s="116"/>
-      <c r="I15" s="116"/>
-      <c r="J15" s="116"/>
-      <c r="K15" s="116"/>
+      <c r="F15" s="140"/>
+      <c r="G15" s="80"/>
+      <c r="H15" s="80"/>
+      <c r="I15" s="80"/>
+      <c r="J15" s="80"/>
+      <c r="K15" s="80"/>
     </row>
     <row r="16" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E16" s="116"/>
-      <c r="F16" s="116"/>
-      <c r="G16" s="116"/>
-      <c r="H16" s="116"/>
-      <c r="I16" s="116"/>
-      <c r="J16" s="116"/>
-      <c r="K16" s="116"/>
+      <c r="E16" s="80"/>
+      <c r="F16" s="80"/>
+      <c r="G16" s="80"/>
+      <c r="H16" s="80"/>
+      <c r="I16" s="80"/>
+      <c r="J16" s="80"/>
+      <c r="K16" s="80"/>
     </row>
     <row r="17" spans="5:29" x14ac:dyDescent="0.25">
       <c r="G17" s="16"/>
@@ -6537,19 +6544,19 @@
       <c r="I17" s="16"/>
     </row>
     <row r="18" spans="5:29" x14ac:dyDescent="0.25">
-      <c r="E18" s="81" t="s">
+      <c r="E18" s="129" t="s">
         <v>122</v>
       </c>
-      <c r="F18" s="81"/>
+      <c r="F18" s="129"/>
     </row>
     <row r="20" spans="5:29" x14ac:dyDescent="0.25">
-      <c r="E20" s="82" t="s">
+      <c r="E20" s="72" t="s">
         <v>123</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="H20" s="83" t="s">
+      <c r="H20" s="73" t="s">
         <v>127</v>
       </c>
       <c r="J20" s="13" t="s">
@@ -6561,303 +6568,303 @@
       <c r="N20" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="P20" s="118" t="s">
+      <c r="P20" s="141" t="s">
         <v>9</v>
       </c>
-      <c r="Q20" s="119"/>
-      <c r="S20" s="118" t="s">
+      <c r="Q20" s="142"/>
+      <c r="S20" s="141" t="s">
         <v>142</v>
       </c>
-      <c r="T20" s="119"/>
-      <c r="V20" s="118" t="s">
+      <c r="T20" s="142"/>
+      <c r="V20" s="141" t="s">
         <v>173</v>
       </c>
-      <c r="W20" s="120"/>
-      <c r="X20" s="119"/>
-      <c r="Z20" s="118" t="s">
+      <c r="W20" s="147"/>
+      <c r="X20" s="142"/>
+      <c r="Z20" s="141" t="s">
         <v>128</v>
       </c>
-      <c r="AA20" s="119"/>
-      <c r="AB20" s="67" t="s">
+      <c r="AA20" s="142"/>
+      <c r="AB20" s="109" t="s">
         <v>129</v>
       </c>
-      <c r="AC20" s="67"/>
+      <c r="AC20" s="109"/>
     </row>
     <row r="25" spans="5:29" x14ac:dyDescent="0.25">
       <c r="N25" s="6"/>
       <c r="O25" s="17"/>
       <c r="P25" s="6"/>
       <c r="Q25" s="17"/>
-      <c r="R25" s="126"/>
-      <c r="S25" s="126"/>
+      <c r="R25" s="82"/>
+      <c r="S25" s="82"/>
     </row>
     <row r="26" spans="5:29" x14ac:dyDescent="0.25">
       <c r="E26" s="27" t="s">
         <v>124</v>
       </c>
-      <c r="F26" s="94" t="s">
+      <c r="F26" s="117" t="s">
         <v>105</v>
       </c>
-      <c r="G26" s="97"/>
-      <c r="H26" s="95" t="s">
+      <c r="G26" s="118"/>
+      <c r="H26" s="146" t="s">
         <v>8</v>
       </c>
-      <c r="I26" s="95"/>
-      <c r="J26" s="95"/>
-      <c r="K26" s="122" t="s">
+      <c r="I26" s="146"/>
+      <c r="J26" s="146"/>
+      <c r="K26" s="81" t="s">
         <v>106</v>
       </c>
-      <c r="L26" s="88" t="s">
+      <c r="L26" s="138" t="s">
         <v>9</v>
       </c>
-      <c r="M26" s="121"/>
-      <c r="N26" s="88" t="s">
+      <c r="M26" s="148"/>
+      <c r="N26" s="138" t="s">
         <v>142</v>
       </c>
-      <c r="O26" s="121"/>
-      <c r="P26" s="143" t="s">
+      <c r="O26" s="148"/>
+      <c r="P26" s="153" t="s">
         <v>174</v>
       </c>
-      <c r="Q26" s="115"/>
-      <c r="R26" s="140"/>
-      <c r="S26" s="126" t="s">
+      <c r="Q26" s="154"/>
+      <c r="R26" s="155"/>
+      <c r="S26" s="82" t="s">
         <v>175</v>
       </c>
-      <c r="T26" s="67" t="s">
+      <c r="T26" s="109" t="s">
         <v>131</v>
       </c>
-      <c r="U26" s="67"/>
+      <c r="U26" s="109"/>
     </row>
     <row r="27" spans="5:29" x14ac:dyDescent="0.25">
       <c r="E27" s="56" t="s">
         <v>179</v>
       </c>
-      <c r="F27" s="88" t="s">
+      <c r="F27" s="138" t="s">
         <v>179</v>
       </c>
-      <c r="G27" s="128"/>
-      <c r="H27" s="86" t="s">
+      <c r="G27" s="139"/>
+      <c r="H27" s="126" t="s">
         <v>179</v>
       </c>
-      <c r="I27" s="90"/>
-      <c r="J27" s="87"/>
+      <c r="I27" s="127"/>
+      <c r="J27" s="128"/>
       <c r="K27" s="56" t="s">
         <v>179</v>
       </c>
-      <c r="L27" s="88" t="s">
+      <c r="L27" s="138" t="s">
         <v>179</v>
       </c>
-      <c r="M27" s="121"/>
-      <c r="N27" s="88" t="s">
+      <c r="M27" s="148"/>
+      <c r="N27" s="138" t="s">
         <v>179</v>
       </c>
-      <c r="O27" s="121"/>
-      <c r="P27" s="110" t="s">
+      <c r="O27" s="148"/>
+      <c r="P27" s="135" t="s">
         <v>179</v>
       </c>
-      <c r="Q27" s="111"/>
-      <c r="R27" s="112"/>
-      <c r="S27" s="127"/>
-      <c r="T27" s="90"/>
-      <c r="U27" s="90"/>
+      <c r="Q27" s="136"/>
+      <c r="R27" s="137"/>
+      <c r="S27" s="83"/>
+      <c r="T27" s="127"/>
+      <c r="U27" s="127"/>
     </row>
     <row r="28" spans="5:29" x14ac:dyDescent="0.25">
-      <c r="E28" s="137">
+      <c r="E28" s="90">
         <v>1</v>
       </c>
-      <c r="F28" s="123">
+      <c r="F28" s="143">
         <v>2021</v>
       </c>
-      <c r="G28" s="124"/>
-      <c r="H28" s="125" t="s">
+      <c r="G28" s="144"/>
+      <c r="H28" s="145" t="s">
         <v>11</v>
       </c>
-      <c r="I28" s="125"/>
-      <c r="J28" s="125"/>
-      <c r="K28" s="129">
+      <c r="I28" s="145"/>
+      <c r="J28" s="145"/>
+      <c r="K28" s="84">
         <v>44196</v>
       </c>
-      <c r="L28" s="130">
+      <c r="L28" s="151">
         <v>2300</v>
       </c>
-      <c r="M28" s="141"/>
-      <c r="N28" s="123" t="s">
+      <c r="M28" s="152"/>
+      <c r="N28" s="143" t="s">
         <v>28</v>
       </c>
-      <c r="O28" s="125"/>
-      <c r="P28" s="123" t="s">
+      <c r="O28" s="145"/>
+      <c r="P28" s="143" t="s">
         <v>89</v>
       </c>
-      <c r="Q28" s="125"/>
-      <c r="R28" s="124"/>
-      <c r="S28" s="139" t="s">
+      <c r="Q28" s="145"/>
+      <c r="R28" s="144"/>
+      <c r="S28" s="92" t="s">
         <v>132</v>
       </c>
-      <c r="T28" s="125" t="s">
+      <c r="T28" s="145" t="s">
         <v>133</v>
       </c>
-      <c r="U28" s="125"/>
+      <c r="U28" s="145"/>
     </row>
     <row r="29" spans="5:29" x14ac:dyDescent="0.25">
-      <c r="E29" s="138">
+      <c r="E29" s="91">
         <v>2</v>
       </c>
-      <c r="F29" s="94">
+      <c r="F29" s="117">
         <v>2021</v>
       </c>
-      <c r="G29" s="95"/>
-      <c r="H29" s="94" t="s">
+      <c r="G29" s="146"/>
+      <c r="H29" s="117" t="s">
         <v>11</v>
       </c>
-      <c r="I29" s="95"/>
-      <c r="J29" s="97"/>
-      <c r="K29" s="131">
+      <c r="I29" s="146"/>
+      <c r="J29" s="118"/>
+      <c r="K29" s="85">
         <v>44198</v>
       </c>
-      <c r="L29" s="132">
+      <c r="L29" s="149">
         <v>750</v>
       </c>
-      <c r="M29" s="142"/>
-      <c r="N29" s="94" t="s">
+      <c r="M29" s="150"/>
+      <c r="N29" s="117" t="s">
         <v>95</v>
       </c>
-      <c r="O29" s="95"/>
-      <c r="P29" s="94" t="s">
+      <c r="O29" s="146"/>
+      <c r="P29" s="117" t="s">
         <v>2</v>
       </c>
-      <c r="Q29" s="95"/>
-      <c r="R29" s="97"/>
-      <c r="S29" s="113" t="s">
+      <c r="Q29" s="146"/>
+      <c r="R29" s="118"/>
+      <c r="S29" s="78" t="s">
         <v>132</v>
       </c>
-      <c r="T29" s="68" t="s">
+      <c r="T29" s="108" t="s">
         <v>133</v>
       </c>
-      <c r="U29" s="68"/>
+      <c r="U29" s="108"/>
     </row>
     <row r="30" spans="5:29" x14ac:dyDescent="0.25">
-      <c r="E30" s="138">
+      <c r="E30" s="91">
         <v>3</v>
       </c>
-      <c r="F30" s="94">
+      <c r="F30" s="117">
         <v>2021</v>
       </c>
-      <c r="G30" s="95"/>
-      <c r="H30" s="94" t="s">
+      <c r="G30" s="146"/>
+      <c r="H30" s="117" t="s">
         <v>11</v>
       </c>
-      <c r="I30" s="95"/>
-      <c r="J30" s="97"/>
-      <c r="K30" s="133"/>
-      <c r="L30" s="132"/>
-      <c r="M30" s="142"/>
-      <c r="N30" s="94"/>
-      <c r="O30" s="95"/>
-      <c r="P30" s="94"/>
-      <c r="Q30" s="95"/>
-      <c r="R30" s="97"/>
-      <c r="S30" s="113" t="s">
+      <c r="I30" s="146"/>
+      <c r="J30" s="118"/>
+      <c r="K30" s="86"/>
+      <c r="L30" s="149"/>
+      <c r="M30" s="150"/>
+      <c r="N30" s="117"/>
+      <c r="O30" s="146"/>
+      <c r="P30" s="117"/>
+      <c r="Q30" s="146"/>
+      <c r="R30" s="118"/>
+      <c r="S30" s="78" t="s">
         <v>132</v>
       </c>
-      <c r="T30" s="68" t="s">
+      <c r="T30" s="108" t="s">
         <v>133</v>
       </c>
-      <c r="U30" s="68"/>
+      <c r="U30" s="108"/>
     </row>
     <row r="31" spans="5:29" x14ac:dyDescent="0.25">
-      <c r="E31" s="138">
+      <c r="E31" s="91">
         <v>4</v>
       </c>
-      <c r="F31" s="94">
+      <c r="F31" s="117">
         <v>2021</v>
       </c>
-      <c r="G31" s="97"/>
-      <c r="H31" s="95" t="s">
+      <c r="G31" s="118"/>
+      <c r="H31" s="146" t="s">
         <v>12</v>
       </c>
-      <c r="I31" s="95"/>
-      <c r="J31" s="95"/>
-      <c r="K31" s="134">
+      <c r="I31" s="146"/>
+      <c r="J31" s="146"/>
+      <c r="K31" s="87">
         <v>44226</v>
       </c>
-      <c r="L31" s="132">
+      <c r="L31" s="149">
         <v>2290</v>
       </c>
-      <c r="M31" s="142"/>
-      <c r="N31" s="94" t="s">
+      <c r="M31" s="150"/>
+      <c r="N31" s="117" t="s">
         <v>28</v>
       </c>
-      <c r="O31" s="95"/>
-      <c r="P31" s="94" t="s">
+      <c r="O31" s="146"/>
+      <c r="P31" s="117" t="s">
         <v>89</v>
       </c>
-      <c r="Q31" s="95"/>
-      <c r="R31" s="97"/>
-      <c r="S31" s="113" t="s">
+      <c r="Q31" s="146"/>
+      <c r="R31" s="118"/>
+      <c r="S31" s="78" t="s">
         <v>132</v>
       </c>
-      <c r="T31" s="68" t="s">
+      <c r="T31" s="108" t="s">
         <v>133</v>
       </c>
-      <c r="U31" s="68"/>
+      <c r="U31" s="108"/>
     </row>
     <row r="32" spans="5:29" x14ac:dyDescent="0.25">
-      <c r="E32" s="138">
+      <c r="E32" s="91">
         <v>5</v>
       </c>
-      <c r="F32" s="94">
+      <c r="F32" s="117">
         <v>2021</v>
       </c>
-      <c r="G32" s="97"/>
-      <c r="H32" s="68" t="s">
+      <c r="G32" s="118"/>
+      <c r="H32" s="108" t="s">
         <v>12</v>
       </c>
-      <c r="I32" s="68"/>
-      <c r="J32" s="68"/>
-      <c r="K32" s="135"/>
-      <c r="L32" s="132"/>
-      <c r="M32" s="142"/>
-      <c r="N32" s="94"/>
-      <c r="O32" s="95"/>
-      <c r="P32" s="94"/>
-      <c r="Q32" s="95"/>
-      <c r="R32" s="97"/>
-      <c r="S32" s="113" t="s">
+      <c r="I32" s="108"/>
+      <c r="J32" s="108"/>
+      <c r="K32" s="88"/>
+      <c r="L32" s="149"/>
+      <c r="M32" s="150"/>
+      <c r="N32" s="117"/>
+      <c r="O32" s="146"/>
+      <c r="P32" s="117"/>
+      <c r="Q32" s="146"/>
+      <c r="R32" s="118"/>
+      <c r="S32" s="78" t="s">
         <v>132</v>
       </c>
-      <c r="T32" s="68" t="s">
+      <c r="T32" s="108" t="s">
         <v>133</v>
       </c>
-      <c r="U32" s="68"/>
+      <c r="U32" s="108"/>
     </row>
     <row r="33" spans="5:21" x14ac:dyDescent="0.25">
-      <c r="E33" s="138">
+      <c r="E33" s="91">
         <v>6</v>
       </c>
-      <c r="F33" s="94">
+      <c r="F33" s="117">
         <v>2021</v>
       </c>
-      <c r="G33" s="97"/>
-      <c r="H33" s="68" t="s">
+      <c r="G33" s="118"/>
+      <c r="H33" s="108" t="s">
         <v>12</v>
       </c>
-      <c r="I33" s="68"/>
-      <c r="J33" s="68"/>
-      <c r="K33" s="135"/>
-      <c r="L33" s="132"/>
-      <c r="M33" s="142"/>
-      <c r="N33" s="94"/>
-      <c r="O33" s="95"/>
-      <c r="P33" s="94"/>
-      <c r="Q33" s="95"/>
-      <c r="R33" s="97"/>
-      <c r="S33" s="113" t="s">
+      <c r="I33" s="108"/>
+      <c r="J33" s="108"/>
+      <c r="K33" s="88"/>
+      <c r="L33" s="149"/>
+      <c r="M33" s="150"/>
+      <c r="N33" s="117"/>
+      <c r="O33" s="146"/>
+      <c r="P33" s="117"/>
+      <c r="Q33" s="146"/>
+      <c r="R33" s="118"/>
+      <c r="S33" s="78" t="s">
         <v>132</v>
       </c>
-      <c r="T33" s="68" t="s">
+      <c r="T33" s="108" t="s">
         <v>133</v>
       </c>
-      <c r="U33" s="68"/>
+      <c r="U33" s="108"/>
     </row>
   </sheetData>
   <mergeCells count="55">
@@ -6866,20 +6873,12 @@
     <mergeCell ref="T31:U31"/>
     <mergeCell ref="T32:U32"/>
     <mergeCell ref="T28:U28"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="L31:M31"/>
+    <mergeCell ref="L32:M32"/>
     <mergeCell ref="F26:G26"/>
     <mergeCell ref="H26:J26"/>
     <mergeCell ref="L26:M26"/>
-    <mergeCell ref="N26:O26"/>
-    <mergeCell ref="P26:R26"/>
-    <mergeCell ref="N29:O29"/>
-    <mergeCell ref="N30:O30"/>
-    <mergeCell ref="N31:O31"/>
-    <mergeCell ref="N32:O32"/>
-    <mergeCell ref="L28:M28"/>
-    <mergeCell ref="L29:M29"/>
-    <mergeCell ref="L30:M30"/>
-    <mergeCell ref="L31:M31"/>
-    <mergeCell ref="L32:M32"/>
     <mergeCell ref="L33:M33"/>
     <mergeCell ref="N33:O33"/>
     <mergeCell ref="P33:R33"/>
@@ -6890,13 +6889,12 @@
     <mergeCell ref="P31:R31"/>
     <mergeCell ref="P32:R32"/>
     <mergeCell ref="N28:O28"/>
-    <mergeCell ref="V20:X20"/>
-    <mergeCell ref="Z20:AA20"/>
-    <mergeCell ref="P27:R27"/>
-    <mergeCell ref="N27:O27"/>
-    <mergeCell ref="L27:M27"/>
-    <mergeCell ref="T27:U27"/>
-    <mergeCell ref="T26:U26"/>
+    <mergeCell ref="N29:O29"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="N31:O31"/>
+    <mergeCell ref="N32:O32"/>
+    <mergeCell ref="L28:M28"/>
+    <mergeCell ref="L29:M29"/>
     <mergeCell ref="F31:G31"/>
     <mergeCell ref="H31:J31"/>
     <mergeCell ref="F32:G32"/>
@@ -6916,6 +6914,15 @@
     <mergeCell ref="E15:F15"/>
     <mergeCell ref="P20:Q20"/>
     <mergeCell ref="S20:T20"/>
+    <mergeCell ref="V20:X20"/>
+    <mergeCell ref="Z20:AA20"/>
+    <mergeCell ref="P27:R27"/>
+    <mergeCell ref="N27:O27"/>
+    <mergeCell ref="L27:M27"/>
+    <mergeCell ref="T27:U27"/>
+    <mergeCell ref="T26:U26"/>
+    <mergeCell ref="N26:O26"/>
+    <mergeCell ref="P26:R26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -6940,10 +6947,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="67" t="s">
+      <c r="A3" s="109" t="s">
         <v>117</v>
       </c>
-      <c r="B3" s="67"/>
+      <c r="B3" s="109"/>
       <c r="N3" t="s">
         <v>113</v>
       </c>
@@ -6955,12 +6962,12 @@
       <c r="E5" s="65"/>
       <c r="F5" s="65"/>
       <c r="G5" s="65"/>
-      <c r="N5" s="77" t="s">
+      <c r="N5" s="159" t="s">
         <v>116</v>
       </c>
-      <c r="O5" s="68"/>
-      <c r="P5" s="68"/>
-      <c r="Q5" s="68"/>
+      <c r="O5" s="108"/>
+      <c r="P5" s="108"/>
+      <c r="Q5" s="108"/>
     </row>
     <row r="6" spans="1:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="65"/>
@@ -6969,13 +6976,13 @@
       <c r="E6" s="65"/>
       <c r="F6" s="65"/>
       <c r="G6" s="65"/>
-      <c r="N6" s="78" t="s">
+      <c r="N6" s="156" t="s">
         <v>118</v>
       </c>
-      <c r="O6" s="79"/>
-      <c r="P6" s="79"/>
-      <c r="Q6" s="79"/>
-      <c r="R6" s="79"/>
+      <c r="O6" s="157"/>
+      <c r="P6" s="157"/>
+      <c r="Q6" s="157"/>
+      <c r="R6" s="157"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="N7" s="36" t="s">
@@ -6986,7 +6993,7 @@
       <c r="N8" s="36" t="s">
         <v>180</v>
       </c>
-      <c r="P8" s="106" t="s">
+      <c r="P8" s="77" t="s">
         <v>181</v>
       </c>
     </row>
@@ -7006,119 +7013,119 @@
       <c r="B11" s="66"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="D12" s="70" t="s">
+      <c r="D12" s="160" t="s">
         <v>107</v>
       </c>
-      <c r="E12" s="70"/>
-      <c r="F12" s="70" t="s">
+      <c r="E12" s="160"/>
+      <c r="F12" s="160" t="s">
         <v>108</v>
       </c>
-      <c r="G12" s="70"/>
-      <c r="H12" s="70" t="s">
+      <c r="G12" s="160"/>
+      <c r="H12" s="160" t="s">
         <v>109</v>
       </c>
-      <c r="I12" s="70"/>
+      <c r="I12" s="160"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="D13" s="70"/>
-      <c r="E13" s="70"/>
-      <c r="F13" s="70"/>
-      <c r="G13" s="70"/>
-      <c r="H13" s="70"/>
-      <c r="I13" s="70"/>
+      <c r="D13" s="160"/>
+      <c r="E13" s="160"/>
+      <c r="F13" s="160"/>
+      <c r="G13" s="160"/>
+      <c r="H13" s="160"/>
+      <c r="I13" s="160"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="D16" s="75" t="s">
+      <c r="D16" s="161" t="s">
         <v>46</v>
       </c>
       <c r="E16" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="F16" s="69">
+      <c r="F16" s="67">
         <v>3623</v>
       </c>
     </row>
     <row r="17" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D17" s="75"/>
+      <c r="D17" s="161"/>
       <c r="E17" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="F17" s="69">
+      <c r="F17" s="67">
         <v>700</v>
       </c>
     </row>
     <row r="18" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D18" s="75"/>
+      <c r="D18" s="161"/>
       <c r="E18" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="F18" s="69">
+      <c r="F18" s="67">
         <v>2000</v>
       </c>
     </row>
     <row r="19" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D19" s="75"/>
-      <c r="E19" s="73" t="s">
+      <c r="D19" s="161"/>
+      <c r="E19" s="70" t="s">
         <v>115</v>
       </c>
-      <c r="F19" s="74">
+      <c r="F19" s="71">
         <f>SUM(F16:F18)</f>
         <v>6323</v>
       </c>
     </row>
     <row r="24" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D24" s="76" t="s">
+      <c r="D24" s="158" t="s">
         <v>6</v>
       </c>
       <c r="E24" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="F24" s="69">
+      <c r="F24" s="67">
         <v>1000</v>
       </c>
     </row>
     <row r="25" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D25" s="76"/>
+      <c r="D25" s="158"/>
       <c r="E25" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="F25" s="69">
+      <c r="F25" s="67">
         <v>300</v>
       </c>
     </row>
     <row r="26" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D26" s="76"/>
+      <c r="D26" s="158"/>
       <c r="E26" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="F26" s="69">
+      <c r="F26" s="67">
         <v>200</v>
       </c>
     </row>
     <row r="27" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D27" s="76"/>
+      <c r="D27" s="158"/>
       <c r="E27" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="F27" s="69">
+      <c r="F27" s="67">
         <v>200</v>
       </c>
     </row>
     <row r="28" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D28" s="76"/>
+      <c r="D28" s="158"/>
       <c r="E28" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="F28" s="69">
+      <c r="F28" s="67">
         <v>500</v>
       </c>
     </row>
     <row r="29" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D29" s="76"/>
-      <c r="E29" s="71" t="s">
+      <c r="D29" s="158"/>
+      <c r="E29" s="68" t="s">
         <v>114</v>
       </c>
-      <c r="F29" s="72">
+      <c r="F29" s="69">
         <f>SUM(F24:F28)</f>
         <v>2200</v>
       </c>
@@ -7127,12 +7134,12 @@
       <c r="B34" t="s">
         <v>145</v>
       </c>
-      <c r="C34" s="106" t="s">
+      <c r="C34" s="77" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C35" s="106" t="s">
+      <c r="C35" s="77" t="s">
         <v>144</v>
       </c>
     </row>
@@ -8269,23 +8276,23 @@
       <c r="D6" t="s">
         <v>63</v>
       </c>
-      <c r="F6" s="68" t="s">
+      <c r="F6" s="108" t="s">
         <v>62</v>
       </c>
-      <c r="G6" s="68"/>
-      <c r="H6" s="68"/>
-      <c r="I6" s="68"/>
+      <c r="G6" s="108"/>
+      <c r="H6" s="108"/>
+      <c r="I6" s="108"/>
       <c r="J6" s="16"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="G8" s="67" t="s">
+      <c r="G8" s="109" t="s">
         <v>63</v>
       </c>
-      <c r="H8" s="67"/>
-      <c r="I8" s="67" t="s">
+      <c r="H8" s="109"/>
+      <c r="I8" s="109" t="s">
         <v>64</v>
       </c>
-      <c r="J8" s="67"/>
+      <c r="J8" s="109"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="60" t="s">
@@ -8891,19 +8898,12 @@
     <mergeCell ref="G8:H8"/>
     <mergeCell ref="I8:J8"/>
   </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J9" xr:uid="{A7489A26-FC2A-465D-B9A6-03692C335CA5}">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A7489A26-FC2A-465D-B9A6-03692C335CA5}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>J9</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -8926,14 +8926,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="109" t="s">
         <v>50</v>
       </c>
-      <c r="B2" s="67"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
+      <c r="B2" s="109"/>
+      <c r="C2" s="109"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="109"/>
+      <c r="F2" s="109"/>
       <c r="G2" s="16"/>
       <c r="H2" s="16"/>
       <c r="I2" s="16"/>
@@ -9551,7 +9551,7 @@
   <dimension ref="B4:U58"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="P24" sqref="P24"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9567,7 +9567,7 @@
     <col min="11" max="11" width="2.140625" customWidth="1"/>
     <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="4.140625" customWidth="1"/>
-    <col min="14" max="14" width="12.42578125" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="20.5703125" bestFit="1" customWidth="1"/>
@@ -9576,13 +9576,13 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="C4" s="67" t="s">
+      <c r="C4" s="109" t="s">
         <v>200</v>
       </c>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
+      <c r="D4" s="109"/>
+      <c r="E4" s="109"/>
+      <c r="F4" s="109"/>
+      <c r="G4" s="109"/>
       <c r="H4">
         <v>2021</v>
       </c>
@@ -9621,7 +9621,7 @@
         <v>11</v>
       </c>
       <c r="E7" s="17"/>
-      <c r="F7" s="69">
+      <c r="F7" s="67">
         <v>187.98</v>
       </c>
       <c r="G7" s="17"/>
@@ -9629,17 +9629,17 @@
       <c r="I7" t="s">
         <v>196</v>
       </c>
-      <c r="L7" s="69">
-        <v>30203</v>
-      </c>
-      <c r="N7" s="147">
+      <c r="L7" s="67">
+        <v>30292.79</v>
+      </c>
+      <c r="N7" s="94">
         <f>F31/L7</f>
-        <v>7.8109459325232583E-2</v>
+        <v>7.7877937291348856E-2</v>
       </c>
       <c r="P7" s="52"/>
-      <c r="Q7" s="116"/>
-      <c r="R7" s="116"/>
-      <c r="S7" s="160"/>
+      <c r="Q7" s="80"/>
+      <c r="R7" s="80"/>
+      <c r="S7" s="106"/>
       <c r="T7" s="52"/>
     </row>
     <row r="8" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -9651,9 +9651,9 @@
       <c r="G8" s="17"/>
       <c r="H8" s="17"/>
       <c r="P8" s="52"/>
-      <c r="Q8" s="116"/>
-      <c r="R8" s="116"/>
-      <c r="S8" s="160"/>
+      <c r="Q8" s="80"/>
+      <c r="R8" s="80"/>
+      <c r="S8" s="106"/>
       <c r="T8" s="52"/>
     </row>
     <row r="9" spans="2:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -9663,32 +9663,32 @@
         <v>12</v>
       </c>
       <c r="E9" s="17"/>
-      <c r="F9" s="69">
+      <c r="F9" s="67">
         <v>198.5</v>
       </c>
       <c r="G9" s="17"/>
       <c r="H9" s="17"/>
-      <c r="I9" s="68" t="s">
+      <c r="I9" s="108" t="s">
         <v>197</v>
       </c>
-      <c r="J9" s="148">
+      <c r="J9" s="112">
         <v>10084</v>
       </c>
-      <c r="L9" s="145">
+      <c r="L9" s="110">
         <f>IF(L7&gt;J9,J9,L7-J9)</f>
         <v>10084</v>
       </c>
-      <c r="M9" s="80" t="s">
+      <c r="M9" s="111" t="s">
         <v>203</v>
       </c>
-      <c r="N9" s="146">
+      <c r="N9" s="113">
         <f>L9*0</f>
         <v>0</v>
       </c>
-      <c r="P9" s="161"/>
-      <c r="Q9" s="116"/>
-      <c r="R9" s="116"/>
-      <c r="S9" s="160"/>
+      <c r="P9" s="107"/>
+      <c r="Q9" s="80"/>
+      <c r="R9" s="80"/>
+      <c r="S9" s="106"/>
       <c r="T9" s="52"/>
     </row>
     <row r="10" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -9699,15 +9699,15 @@
       <c r="F10" s="21"/>
       <c r="G10" s="17"/>
       <c r="H10" s="17"/>
-      <c r="I10" s="68"/>
-      <c r="J10" s="148"/>
-      <c r="L10" s="67"/>
-      <c r="M10" s="67"/>
-      <c r="N10" s="68"/>
+      <c r="I10" s="108"/>
+      <c r="J10" s="112"/>
+      <c r="L10" s="109"/>
+      <c r="M10" s="109"/>
+      <c r="N10" s="108"/>
       <c r="P10" s="52"/>
-      <c r="Q10" s="116"/>
-      <c r="R10" s="116"/>
-      <c r="S10" s="160"/>
+      <c r="Q10" s="80"/>
+      <c r="R10" s="80"/>
+      <c r="S10" s="106"/>
       <c r="T10" s="52"/>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
@@ -9717,32 +9717,32 @@
         <v>13</v>
       </c>
       <c r="E11" s="17"/>
-      <c r="F11" s="69">
+      <c r="F11" s="67">
         <v>198.5</v>
       </c>
       <c r="G11" s="17"/>
       <c r="H11" s="17"/>
-      <c r="I11" s="68" t="s">
+      <c r="I11" s="108" t="s">
         <v>198</v>
       </c>
-      <c r="J11" s="148">
+      <c r="J11" s="112">
         <v>25710</v>
       </c>
-      <c r="L11" s="145">
-        <f>IF(L7&gt;J11,J11,L7-L9)</f>
-        <v>25710</v>
-      </c>
-      <c r="M11" s="80" t="s">
+      <c r="L11" s="110">
+        <f>IF(L7&gt;(J9+J11),J11,L7-L9)</f>
+        <v>20208.79</v>
+      </c>
+      <c r="M11" s="111" t="s">
         <v>203</v>
       </c>
-      <c r="N11" s="146">
+      <c r="N11" s="113">
         <f>L11*11%</f>
-        <v>2828.1</v>
+        <v>2222.9668999999999</v>
       </c>
       <c r="P11" s="52"/>
-      <c r="Q11" s="116"/>
-      <c r="R11" s="116"/>
-      <c r="S11" s="160"/>
+      <c r="Q11" s="80"/>
+      <c r="R11" s="80"/>
+      <c r="S11" s="106"/>
       <c r="T11" s="52"/>
     </row>
     <row r="12" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -9753,15 +9753,15 @@
       <c r="F12" s="21"/>
       <c r="G12" s="17"/>
       <c r="H12" s="17"/>
-      <c r="I12" s="68"/>
-      <c r="J12" s="148"/>
-      <c r="L12" s="67"/>
-      <c r="M12" s="67"/>
-      <c r="N12" s="68"/>
+      <c r="I12" s="108"/>
+      <c r="J12" s="112"/>
+      <c r="L12" s="109"/>
+      <c r="M12" s="109"/>
+      <c r="N12" s="108"/>
       <c r="P12" s="52"/>
-      <c r="Q12" s="116"/>
-      <c r="R12" s="116"/>
-      <c r="S12" s="160"/>
+      <c r="Q12" s="80"/>
+      <c r="R12" s="80"/>
+      <c r="S12" s="106"/>
       <c r="T12" s="52"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
@@ -9771,32 +9771,32 @@
         <v>14</v>
       </c>
       <c r="E13" s="17"/>
-      <c r="F13" s="69">
+      <c r="F13" s="67">
         <v>198.5</v>
       </c>
       <c r="G13" s="17"/>
       <c r="H13" s="17"/>
-      <c r="I13" s="68" t="s">
+      <c r="I13" s="108" t="s">
         <v>199</v>
       </c>
-      <c r="J13" s="148">
+      <c r="J13" s="112">
         <v>73516</v>
       </c>
-      <c r="L13" s="145">
-        <f>IF(L7&gt;J13,J13,L7-L9-L11)</f>
-        <v>-5591</v>
-      </c>
-      <c r="M13" s="80" t="s">
+      <c r="L13" s="110">
+        <f>IF(L7&gt;(J9+J11+J13),J13,L7-L9-L11)</f>
+        <v>0</v>
+      </c>
+      <c r="M13" s="111" t="s">
         <v>203</v>
       </c>
-      <c r="N13" s="146">
+      <c r="N13" s="113">
         <f>L13*30%</f>
-        <v>-1677.3</v>
+        <v>0</v>
       </c>
       <c r="P13" s="52"/>
-      <c r="Q13" s="116"/>
-      <c r="R13" s="116"/>
-      <c r="S13" s="160"/>
+      <c r="Q13" s="80"/>
+      <c r="R13" s="80"/>
+      <c r="S13" s="106"/>
       <c r="T13" s="52"/>
     </row>
     <row r="14" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -9807,15 +9807,15 @@
       <c r="F14" s="21"/>
       <c r="G14" s="17"/>
       <c r="H14" s="17"/>
-      <c r="I14" s="68"/>
-      <c r="J14" s="148"/>
-      <c r="L14" s="67"/>
-      <c r="M14" s="67"/>
-      <c r="N14" s="68"/>
+      <c r="I14" s="108"/>
+      <c r="J14" s="112"/>
+      <c r="L14" s="109"/>
+      <c r="M14" s="109"/>
+      <c r="N14" s="108"/>
       <c r="P14" s="52"/>
-      <c r="Q14" s="116"/>
-      <c r="R14" s="116"/>
-      <c r="S14" s="116"/>
+      <c r="Q14" s="80"/>
+      <c r="R14" s="80"/>
+      <c r="S14" s="80"/>
       <c r="T14" s="52"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
@@ -9825,32 +9825,32 @@
         <v>15</v>
       </c>
       <c r="E15" s="17"/>
-      <c r="F15" s="69">
+      <c r="F15" s="67">
         <v>198.5</v>
       </c>
       <c r="G15" s="17"/>
       <c r="H15" s="17"/>
-      <c r="I15" s="68" t="s">
+      <c r="I15" s="108" t="s">
         <v>201</v>
       </c>
-      <c r="J15" s="148">
+      <c r="J15" s="112">
         <v>158122</v>
       </c>
-      <c r="L15" s="145">
-        <f>IF(L7&gt;J15,J15,L7-L9-L11-L13)</f>
+      <c r="L15" s="110">
+        <f>IF(L7&gt;(J9+J11+J13+J15),J15,L7-L9-L11-L13)</f>
         <v>0</v>
       </c>
-      <c r="M15" s="80" t="s">
+      <c r="M15" s="111" t="s">
         <v>203</v>
       </c>
-      <c r="N15" s="146">
+      <c r="N15" s="113">
         <f>L15*41%</f>
         <v>0</v>
       </c>
       <c r="P15" s="52"/>
-      <c r="Q15" s="116"/>
-      <c r="R15" s="116"/>
-      <c r="S15" s="160"/>
+      <c r="Q15" s="80"/>
+      <c r="R15" s="80"/>
+      <c r="S15" s="106"/>
       <c r="T15" s="52"/>
     </row>
     <row r="16" spans="2:20" ht="8.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -9861,15 +9861,15 @@
       <c r="F16" s="21"/>
       <c r="G16" s="17"/>
       <c r="H16" s="17"/>
-      <c r="I16" s="68"/>
-      <c r="J16" s="148"/>
-      <c r="L16" s="67"/>
-      <c r="M16" s="67"/>
-      <c r="N16" s="68"/>
+      <c r="I16" s="108"/>
+      <c r="J16" s="112"/>
+      <c r="L16" s="109"/>
+      <c r="M16" s="109"/>
+      <c r="N16" s="108"/>
       <c r="P16" s="52"/>
-      <c r="Q16" s="116"/>
-      <c r="R16" s="116"/>
-      <c r="S16" s="116"/>
+      <c r="Q16" s="80"/>
+      <c r="R16" s="80"/>
+      <c r="S16" s="80"/>
       <c r="T16" s="52"/>
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.25">
@@ -9879,23 +9879,23 @@
         <v>16</v>
       </c>
       <c r="E17" s="17"/>
-      <c r="F17" s="69">
+      <c r="F17" s="67">
         <v>198.5</v>
       </c>
       <c r="G17" s="17"/>
       <c r="H17" s="17"/>
-      <c r="I17" s="68" t="s">
+      <c r="I17" s="108" t="s">
         <v>202</v>
       </c>
-      <c r="J17" s="148"/>
-      <c r="L17" s="145">
-        <f t="shared" ref="L17" si="0">IF($L$7&gt;J17,J17,$L$7-L15)</f>
+      <c r="J17" s="112"/>
+      <c r="L17" s="110">
+        <f>IF($L$7&gt;(J9+J11+J13+J15+J17),$L$7-L9-L11-L13-L15,0)</f>
         <v>0</v>
       </c>
-      <c r="M17" s="80" t="s">
+      <c r="M17" s="111" t="s">
         <v>203</v>
       </c>
-      <c r="N17" s="146">
+      <c r="N17" s="113">
         <f>L17*45%</f>
         <v>0</v>
       </c>
@@ -9913,11 +9913,11 @@
       <c r="F18" s="21"/>
       <c r="G18" s="17"/>
       <c r="H18" s="17"/>
-      <c r="I18" s="68"/>
-      <c r="J18" s="148"/>
-      <c r="L18" s="67"/>
-      <c r="M18" s="67"/>
-      <c r="N18" s="68"/>
+      <c r="I18" s="108"/>
+      <c r="J18" s="112"/>
+      <c r="L18" s="109"/>
+      <c r="M18" s="109"/>
+      <c r="N18" s="108"/>
       <c r="P18" s="52"/>
       <c r="Q18" s="52"/>
       <c r="R18" s="52"/>
@@ -9931,16 +9931,16 @@
         <v>17</v>
       </c>
       <c r="E19" s="17"/>
-      <c r="F19" s="69">
+      <c r="F19" s="67">
         <v>198.5</v>
       </c>
       <c r="G19" s="17"/>
       <c r="H19" s="17"/>
-      <c r="I19" s="67"/>
+      <c r="I19" s="109"/>
       <c r="J19" s="63"/>
       <c r="N19" s="23">
         <f>SUM(N9:N18)</f>
-        <v>1150.8</v>
+        <v>2222.9668999999999</v>
       </c>
       <c r="P19" s="52"/>
       <c r="Q19" s="52"/>
@@ -9956,7 +9956,7 @@
       <c r="F20" s="21"/>
       <c r="G20" s="17"/>
       <c r="H20" s="17"/>
-      <c r="I20" s="67"/>
+      <c r="I20" s="109"/>
       <c r="J20" s="63"/>
       <c r="P20" s="52"/>
       <c r="Q20" s="52"/>
@@ -9971,7 +9971,7 @@
         <v>18</v>
       </c>
       <c r="E21" s="17"/>
-      <c r="F21" s="69">
+      <c r="F21" s="67">
         <v>187.98</v>
       </c>
       <c r="G21" s="17"/>
@@ -10003,7 +10003,7 @@
         <v>19</v>
       </c>
       <c r="E23" s="17"/>
-      <c r="F23" s="69">
+      <c r="F23" s="67">
         <v>203.5</v>
       </c>
       <c r="G23" s="17"/>
@@ -10035,7 +10035,7 @@
         <v>20</v>
       </c>
       <c r="E25" s="17"/>
-      <c r="F25" s="69">
+      <c r="F25" s="67">
         <v>212.7</v>
       </c>
       <c r="G25" s="17"/>
@@ -10057,7 +10057,7 @@
         <v>21</v>
       </c>
       <c r="E27" s="17"/>
-      <c r="F27" s="69">
+      <c r="F27" s="67">
         <v>187.98</v>
       </c>
       <c r="G27" s="17"/>
@@ -10079,7 +10079,7 @@
         <v>22</v>
       </c>
       <c r="E29" s="17"/>
-      <c r="F29" s="69">
+      <c r="F29" s="67">
         <v>188</v>
       </c>
       <c r="G29" s="17"/>
@@ -10114,254 +10114,254 @@
       <c r="H32" s="17"/>
     </row>
     <row r="37" spans="14:21" x14ac:dyDescent="0.25">
-      <c r="N37" s="149"/>
-      <c r="O37" s="149"/>
-      <c r="P37" s="150"/>
-      <c r="Q37" s="149"/>
-      <c r="R37" s="151"/>
-      <c r="S37" s="150"/>
-      <c r="T37" s="152"/>
-      <c r="U37" s="153"/>
+      <c r="N37" s="95"/>
+      <c r="O37" s="95"/>
+      <c r="P37" s="96"/>
+      <c r="Q37" s="95"/>
+      <c r="R37" s="97"/>
+      <c r="S37" s="96"/>
+      <c r="T37" s="98"/>
+      <c r="U37" s="99"/>
     </row>
     <row r="38" spans="14:21" x14ac:dyDescent="0.25">
-      <c r="N38" s="150"/>
-      <c r="O38" s="150"/>
-      <c r="P38" s="150"/>
-      <c r="Q38" s="150"/>
-      <c r="R38" s="150"/>
-      <c r="S38" s="150"/>
-      <c r="T38" s="151"/>
-      <c r="U38" s="150"/>
+      <c r="N38" s="96"/>
+      <c r="O38" s="96"/>
+      <c r="P38" s="96"/>
+      <c r="Q38" s="96"/>
+      <c r="R38" s="96"/>
+      <c r="S38" s="96"/>
+      <c r="T38" s="97"/>
+      <c r="U38" s="96"/>
     </row>
     <row r="39" spans="14:21" x14ac:dyDescent="0.25">
-      <c r="N39" s="154"/>
-      <c r="O39" s="154"/>
-      <c r="P39" s="150"/>
-      <c r="Q39" s="149"/>
-      <c r="R39" s="152"/>
-      <c r="S39" s="151"/>
-      <c r="T39" s="155"/>
-      <c r="U39" s="151"/>
+      <c r="N39" s="100"/>
+      <c r="O39" s="100"/>
+      <c r="P39" s="96"/>
+      <c r="Q39" s="95"/>
+      <c r="R39" s="98"/>
+      <c r="S39" s="97"/>
+      <c r="T39" s="101"/>
+      <c r="U39" s="97"/>
     </row>
     <row r="40" spans="14:21" x14ac:dyDescent="0.25">
-      <c r="N40" s="154"/>
-      <c r="O40" s="154"/>
-      <c r="P40" s="150"/>
-      <c r="Q40" s="149"/>
-      <c r="R40" s="152"/>
-      <c r="S40" s="151"/>
-      <c r="T40" s="155"/>
-      <c r="U40" s="151"/>
+      <c r="N40" s="100"/>
+      <c r="O40" s="100"/>
+      <c r="P40" s="96"/>
+      <c r="Q40" s="95"/>
+      <c r="R40" s="98"/>
+      <c r="S40" s="97"/>
+      <c r="T40" s="101"/>
+      <c r="U40" s="97"/>
     </row>
     <row r="41" spans="14:21" x14ac:dyDescent="0.25">
-      <c r="N41" s="154"/>
-      <c r="O41" s="154"/>
-      <c r="P41" s="150"/>
-      <c r="Q41" s="149"/>
-      <c r="R41" s="152"/>
-      <c r="S41" s="150"/>
-      <c r="T41" s="155"/>
-      <c r="U41" s="151"/>
+      <c r="N41" s="100"/>
+      <c r="O41" s="100"/>
+      <c r="P41" s="96"/>
+      <c r="Q41" s="95"/>
+      <c r="R41" s="98"/>
+      <c r="S41" s="96"/>
+      <c r="T41" s="101"/>
+      <c r="U41" s="97"/>
     </row>
     <row r="42" spans="14:21" x14ac:dyDescent="0.25">
-      <c r="N42" s="154"/>
-      <c r="O42" s="154"/>
-      <c r="P42" s="150"/>
-      <c r="Q42" s="156"/>
-      <c r="R42" s="157"/>
-      <c r="S42" s="157"/>
-      <c r="T42" s="157"/>
-      <c r="U42" s="151"/>
+      <c r="N42" s="100"/>
+      <c r="O42" s="100"/>
+      <c r="P42" s="96"/>
+      <c r="Q42" s="102"/>
+      <c r="R42" s="103"/>
+      <c r="S42" s="103"/>
+      <c r="T42" s="103"/>
+      <c r="U42" s="97"/>
     </row>
     <row r="43" spans="14:21" x14ac:dyDescent="0.25">
-      <c r="N43" s="154"/>
-      <c r="O43" s="154"/>
-      <c r="P43" s="150"/>
-      <c r="Q43" s="151"/>
-      <c r="R43" s="150"/>
-      <c r="S43" s="153"/>
-      <c r="T43" s="150"/>
-      <c r="U43" s="150"/>
+      <c r="N43" s="100"/>
+      <c r="O43" s="100"/>
+      <c r="P43" s="96"/>
+      <c r="Q43" s="97"/>
+      <c r="R43" s="96"/>
+      <c r="S43" s="99"/>
+      <c r="T43" s="96"/>
+      <c r="U43" s="96"/>
     </row>
     <row r="44" spans="14:21" x14ac:dyDescent="0.25">
-      <c r="N44" s="150"/>
-      <c r="O44" s="150"/>
-      <c r="P44" s="150"/>
-      <c r="Q44" s="151"/>
-      <c r="R44" s="150"/>
-      <c r="S44" s="153"/>
-      <c r="T44" s="150"/>
-      <c r="U44" s="150"/>
+      <c r="N44" s="96"/>
+      <c r="O44" s="96"/>
+      <c r="P44" s="96"/>
+      <c r="Q44" s="97"/>
+      <c r="R44" s="96"/>
+      <c r="S44" s="99"/>
+      <c r="T44" s="96"/>
+      <c r="U44" s="96"/>
     </row>
     <row r="45" spans="14:21" x14ac:dyDescent="0.25">
-      <c r="N45" s="149"/>
-      <c r="O45" s="149"/>
-      <c r="P45" s="150"/>
-      <c r="Q45" s="150"/>
-      <c r="R45" s="150"/>
-      <c r="S45" s="150"/>
-      <c r="T45" s="150"/>
-      <c r="U45" s="150"/>
+      <c r="N45" s="95"/>
+      <c r="O45" s="95"/>
+      <c r="P45" s="96"/>
+      <c r="Q45" s="96"/>
+      <c r="R45" s="96"/>
+      <c r="S45" s="96"/>
+      <c r="T45" s="96"/>
+      <c r="U45" s="96"/>
     </row>
     <row r="46" spans="14:21" x14ac:dyDescent="0.25">
-      <c r="N46" s="149"/>
-      <c r="O46" s="158"/>
-      <c r="P46" s="150"/>
-      <c r="Q46" s="150"/>
-      <c r="R46" s="150"/>
-      <c r="S46" s="150"/>
-      <c r="T46" s="150"/>
-      <c r="U46" s="150"/>
+      <c r="N46" s="95"/>
+      <c r="O46" s="104"/>
+      <c r="P46" s="96"/>
+      <c r="Q46" s="96"/>
+      <c r="R46" s="96"/>
+      <c r="S46" s="96"/>
+      <c r="T46" s="96"/>
+      <c r="U46" s="96"/>
     </row>
     <row r="47" spans="14:21" x14ac:dyDescent="0.25">
-      <c r="N47" s="149"/>
-      <c r="O47" s="158"/>
-      <c r="P47" s="150"/>
-      <c r="Q47" s="150"/>
-      <c r="R47" s="150"/>
-      <c r="S47" s="150"/>
-      <c r="T47" s="150"/>
-      <c r="U47" s="150"/>
+      <c r="N47" s="95"/>
+      <c r="O47" s="104"/>
+      <c r="P47" s="96"/>
+      <c r="Q47" s="96"/>
+      <c r="R47" s="96"/>
+      <c r="S47" s="96"/>
+      <c r="T47" s="96"/>
+      <c r="U47" s="96"/>
     </row>
     <row r="48" spans="14:21" x14ac:dyDescent="0.25">
-      <c r="N48" s="149"/>
-      <c r="O48" s="158"/>
-      <c r="P48" s="150"/>
-      <c r="Q48" s="150"/>
-      <c r="R48" s="150"/>
-      <c r="S48" s="150"/>
-      <c r="T48" s="150"/>
-      <c r="U48" s="150"/>
+      <c r="N48" s="95"/>
+      <c r="O48" s="104"/>
+      <c r="P48" s="96"/>
+      <c r="Q48" s="96"/>
+      <c r="R48" s="96"/>
+      <c r="S48" s="96"/>
+      <c r="T48" s="96"/>
+      <c r="U48" s="96"/>
     </row>
     <row r="49" spans="14:21" x14ac:dyDescent="0.25">
-      <c r="N49" s="149"/>
-      <c r="O49" s="158"/>
-      <c r="P49" s="150"/>
-      <c r="Q49" s="150"/>
-      <c r="R49" s="150"/>
-      <c r="S49" s="150"/>
-      <c r="T49" s="151"/>
-      <c r="U49" s="150"/>
+      <c r="N49" s="95"/>
+      <c r="O49" s="104"/>
+      <c r="P49" s="96"/>
+      <c r="Q49" s="96"/>
+      <c r="R49" s="96"/>
+      <c r="S49" s="96"/>
+      <c r="T49" s="97"/>
+      <c r="U49" s="96"/>
     </row>
     <row r="50" spans="14:21" x14ac:dyDescent="0.25">
-      <c r="N50" s="149"/>
-      <c r="O50" s="158"/>
-      <c r="P50" s="150"/>
-      <c r="Q50" s="150"/>
-      <c r="R50" s="150"/>
-      <c r="S50" s="150"/>
-      <c r="T50" s="151"/>
-      <c r="U50" s="150"/>
+      <c r="N50" s="95"/>
+      <c r="O50" s="104"/>
+      <c r="P50" s="96"/>
+      <c r="Q50" s="96"/>
+      <c r="R50" s="96"/>
+      <c r="S50" s="96"/>
+      <c r="T50" s="97"/>
+      <c r="U50" s="96"/>
     </row>
     <row r="51" spans="14:21" x14ac:dyDescent="0.25">
-      <c r="N51" s="149"/>
-      <c r="O51" s="158"/>
-      <c r="P51" s="150"/>
-      <c r="Q51" s="150"/>
-      <c r="R51" s="150"/>
-      <c r="S51" s="150"/>
-      <c r="T51" s="151"/>
-      <c r="U51" s="150"/>
+      <c r="N51" s="95"/>
+      <c r="O51" s="104"/>
+      <c r="P51" s="96"/>
+      <c r="Q51" s="96"/>
+      <c r="R51" s="96"/>
+      <c r="S51" s="96"/>
+      <c r="T51" s="97"/>
+      <c r="U51" s="96"/>
     </row>
     <row r="52" spans="14:21" x14ac:dyDescent="0.25">
-      <c r="N52" s="149"/>
-      <c r="O52" s="158"/>
-      <c r="P52" s="150"/>
-      <c r="Q52" s="150"/>
-      <c r="R52" s="150"/>
-      <c r="S52" s="150"/>
-      <c r="T52" s="151"/>
-      <c r="U52" s="150"/>
+      <c r="N52" s="95"/>
+      <c r="O52" s="104"/>
+      <c r="P52" s="96"/>
+      <c r="Q52" s="96"/>
+      <c r="R52" s="96"/>
+      <c r="S52" s="96"/>
+      <c r="T52" s="97"/>
+      <c r="U52" s="96"/>
     </row>
     <row r="53" spans="14:21" x14ac:dyDescent="0.25">
-      <c r="N53" s="149"/>
-      <c r="O53" s="158"/>
-      <c r="P53" s="150"/>
-      <c r="Q53" s="150"/>
-      <c r="R53" s="150"/>
-      <c r="S53" s="150"/>
-      <c r="T53" s="151"/>
-      <c r="U53" s="150"/>
+      <c r="N53" s="95"/>
+      <c r="O53" s="104"/>
+      <c r="P53" s="96"/>
+      <c r="Q53" s="96"/>
+      <c r="R53" s="96"/>
+      <c r="S53" s="96"/>
+      <c r="T53" s="97"/>
+      <c r="U53" s="96"/>
     </row>
     <row r="54" spans="14:21" x14ac:dyDescent="0.25">
-      <c r="N54" s="149"/>
-      <c r="O54" s="158"/>
-      <c r="P54" s="150"/>
-      <c r="Q54" s="150"/>
-      <c r="R54" s="150"/>
-      <c r="S54" s="150"/>
-      <c r="T54" s="151"/>
-      <c r="U54" s="150"/>
+      <c r="N54" s="95"/>
+      <c r="O54" s="104"/>
+      <c r="P54" s="96"/>
+      <c r="Q54" s="96"/>
+      <c r="R54" s="96"/>
+      <c r="S54" s="96"/>
+      <c r="T54" s="97"/>
+      <c r="U54" s="96"/>
     </row>
     <row r="55" spans="14:21" x14ac:dyDescent="0.25">
-      <c r="N55" s="149"/>
-      <c r="O55" s="158"/>
-      <c r="P55" s="150"/>
-      <c r="Q55" s="150"/>
-      <c r="R55" s="150"/>
-      <c r="S55" s="150"/>
-      <c r="T55" s="151"/>
-      <c r="U55" s="150"/>
+      <c r="N55" s="95"/>
+      <c r="O55" s="104"/>
+      <c r="P55" s="96"/>
+      <c r="Q55" s="96"/>
+      <c r="R55" s="96"/>
+      <c r="S55" s="96"/>
+      <c r="T55" s="97"/>
+      <c r="U55" s="96"/>
     </row>
     <row r="56" spans="14:21" x14ac:dyDescent="0.25">
-      <c r="N56" s="149"/>
-      <c r="O56" s="158"/>
-      <c r="P56" s="150"/>
-      <c r="Q56" s="150"/>
-      <c r="R56" s="150"/>
-      <c r="S56" s="150"/>
-      <c r="T56" s="151"/>
-      <c r="U56" s="150"/>
+      <c r="N56" s="95"/>
+      <c r="O56" s="104"/>
+      <c r="P56" s="96"/>
+      <c r="Q56" s="96"/>
+      <c r="R56" s="96"/>
+      <c r="S56" s="96"/>
+      <c r="T56" s="97"/>
+      <c r="U56" s="96"/>
     </row>
     <row r="57" spans="14:21" x14ac:dyDescent="0.25">
-      <c r="N57" s="149"/>
-      <c r="O57" s="158"/>
-      <c r="P57" s="150"/>
-      <c r="Q57" s="150"/>
-      <c r="R57" s="150"/>
-      <c r="S57" s="150"/>
-      <c r="T57" s="151"/>
-      <c r="U57" s="150"/>
+      <c r="N57" s="95"/>
+      <c r="O57" s="104"/>
+      <c r="P57" s="96"/>
+      <c r="Q57" s="96"/>
+      <c r="R57" s="96"/>
+      <c r="S57" s="96"/>
+      <c r="T57" s="97"/>
+      <c r="U57" s="96"/>
     </row>
     <row r="58" spans="14:21" x14ac:dyDescent="0.25">
-      <c r="N58" s="149"/>
-      <c r="O58" s="159"/>
-      <c r="P58" s="150"/>
-      <c r="Q58" s="150"/>
-      <c r="R58" s="150"/>
-      <c r="S58" s="150"/>
-      <c r="T58" s="151"/>
-      <c r="U58" s="150"/>
+      <c r="N58" s="95"/>
+      <c r="O58" s="105"/>
+      <c r="P58" s="96"/>
+      <c r="Q58" s="96"/>
+      <c r="R58" s="96"/>
+      <c r="S58" s="96"/>
+      <c r="T58" s="97"/>
+      <c r="U58" s="96"/>
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="J17:J18"/>
     <mergeCell ref="N9:N10"/>
     <mergeCell ref="N11:N12"/>
     <mergeCell ref="N13:N14"/>
     <mergeCell ref="N15:N16"/>
     <mergeCell ref="N17:N18"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="L13:L14"/>
-    <mergeCell ref="L15:L16"/>
-    <mergeCell ref="L17:L18"/>
     <mergeCell ref="M9:M10"/>
     <mergeCell ref="M11:M12"/>
     <mergeCell ref="M13:M14"/>
     <mergeCell ref="M15:M16"/>
     <mergeCell ref="M17:M18"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="L11:L12"/>
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="I11:I12"/>
     <mergeCell ref="I13:I14"/>
     <mergeCell ref="I15:I16"/>
     <mergeCell ref="L9:L10"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="L13:L14"/>
+    <mergeCell ref="L15:L16"/>
+    <mergeCell ref="L17:L18"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="J15:J16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -10393,11 +10393,11 @@
       <c r="B10" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="144" t="s">
+      <c r="C10" s="93" t="s">
         <v>146</v>
       </c>
-      <c r="D10" s="144"/>
-      <c r="E10" s="144"/>
+      <c r="D10" s="93"/>
+      <c r="E10" s="93"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
@@ -10416,11 +10416,11 @@
       <c r="B13" t="s">
         <v>70</v>
       </c>
-      <c r="C13" s="144" t="s">
+      <c r="C13" s="93" t="s">
         <v>185</v>
       </c>
-      <c r="D13" s="144"/>
-      <c r="E13" s="144"/>
+      <c r="D13" s="93"/>
+      <c r="E13" s="93"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
@@ -10474,7 +10474,7 @@
       <c r="B2" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="136" t="s">
+      <c r="F2" s="89" t="s">
         <v>194</v>
       </c>
       <c r="G2" s="64">
@@ -10482,19 +10482,19 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="136" t="s">
+      <c r="B4" s="89" t="s">
         <v>193</v>
       </c>
       <c r="C4" t="s">
         <v>190</v>
       </c>
-      <c r="D4" s="136" t="s">
+      <c r="D4" s="89" t="s">
         <v>193</v>
       </c>
       <c r="E4" t="s">
         <v>191</v>
       </c>
-      <c r="F4" s="136" t="s">
+      <c r="F4" s="89" t="s">
         <v>193</v>
       </c>
       <c r="G4" t="s">
@@ -10502,9 +10502,9 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="67"/>
-      <c r="B7" s="67"/>
-      <c r="C7" s="67"/>
+      <c r="A7" s="109"/>
+      <c r="B7" s="109"/>
+      <c r="C7" s="109"/>
       <c r="H7" t="s">
         <v>189</v>
       </c>
@@ -11256,34 +11256,34 @@
   </cols>
   <sheetData>
     <row r="12" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E12" s="68" t="s">
+      <c r="E12" s="108" t="s">
         <v>195</v>
       </c>
-      <c r="F12" s="68"/>
+      <c r="F12" s="108"/>
     </row>
     <row r="15" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E15" s="100" t="s">
+      <c r="E15" s="119" t="s">
         <v>120</v>
       </c>
-      <c r="F15" s="102"/>
-      <c r="G15" s="84" t="s">
+      <c r="F15" s="120"/>
+      <c r="G15" s="123" t="s">
         <v>119</v>
       </c>
-      <c r="H15" s="89"/>
-      <c r="I15" s="85"/>
-      <c r="J15" s="89" t="s">
+      <c r="H15" s="124"/>
+      <c r="I15" s="125"/>
+      <c r="J15" s="124" t="s">
         <v>121</v>
       </c>
-      <c r="K15" s="85"/>
+      <c r="K15" s="125"/>
     </row>
     <row r="16" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E16" s="103"/>
-      <c r="F16" s="105"/>
-      <c r="G16" s="86"/>
-      <c r="H16" s="90"/>
-      <c r="I16" s="87"/>
-      <c r="J16" s="90"/>
-      <c r="K16" s="87"/>
+      <c r="E16" s="121"/>
+      <c r="F16" s="122"/>
+      <c r="G16" s="126"/>
+      <c r="H16" s="127"/>
+      <c r="I16" s="128"/>
+      <c r="J16" s="127"/>
+      <c r="K16" s="128"/>
     </row>
     <row r="17" spans="5:17" x14ac:dyDescent="0.25">
       <c r="G17" s="16"/>
@@ -11291,19 +11291,19 @@
       <c r="I17" s="16"/>
     </row>
     <row r="18" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E18" s="81" t="s">
+      <c r="E18" s="129" t="s">
         <v>122</v>
       </c>
-      <c r="F18" s="81"/>
+      <c r="F18" s="129"/>
     </row>
     <row r="20" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E20" s="82" t="s">
+      <c r="E20" s="72" t="s">
         <v>123</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="H20" s="83" t="s">
+      <c r="H20" s="73" t="s">
         <v>127</v>
       </c>
       <c r="J20" s="13" t="s">
@@ -11315,28 +11315,28 @@
       <c r="N20" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="P20" s="67" t="s">
+      <c r="P20" s="109" t="s">
         <v>129</v>
       </c>
-      <c r="Q20" s="67"/>
+      <c r="Q20" s="109"/>
     </row>
     <row r="24" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E24" s="114" t="s">
+      <c r="E24" s="79" t="s">
         <v>124</v>
       </c>
-      <c r="F24" s="93" t="s">
+      <c r="F24" s="114" t="s">
         <v>125</v>
       </c>
-      <c r="G24" s="96"/>
-      <c r="H24" s="91" t="s">
+      <c r="G24" s="115"/>
+      <c r="H24" s="116" t="s">
         <v>126</v>
       </c>
-      <c r="I24" s="91"/>
-      <c r="J24" s="91"/>
-      <c r="K24" s="98" t="s">
+      <c r="I24" s="116"/>
+      <c r="J24" s="116"/>
+      <c r="K24" s="75" t="s">
         <v>130</v>
       </c>
-      <c r="L24" s="92" t="s">
+      <c r="L24" s="74" t="s">
         <v>131</v>
       </c>
       <c r="N24" s="16"/>
@@ -11346,16 +11346,16 @@
       <c r="E25">
         <v>1</v>
       </c>
-      <c r="F25" s="94" t="s">
+      <c r="F25" s="117" t="s">
         <v>28</v>
       </c>
-      <c r="G25" s="97"/>
-      <c r="H25" s="68" t="s">
+      <c r="G25" s="118"/>
+      <c r="H25" s="108" t="s">
         <v>24</v>
       </c>
-      <c r="I25" s="68"/>
-      <c r="J25" s="68"/>
-      <c r="K25" s="99" t="s">
+      <c r="I25" s="108"/>
+      <c r="J25" s="108"/>
+      <c r="K25" s="76" t="s">
         <v>132</v>
       </c>
       <c r="L25" s="16" t="s">
@@ -11368,16 +11368,16 @@
       <c r="E26">
         <v>2</v>
       </c>
-      <c r="F26" s="94" t="s">
+      <c r="F26" s="117" t="s">
         <v>95</v>
       </c>
-      <c r="G26" s="97"/>
-      <c r="H26" s="68" t="s">
+      <c r="G26" s="118"/>
+      <c r="H26" s="108" t="s">
         <v>137</v>
       </c>
-      <c r="I26" s="68"/>
-      <c r="J26" s="68"/>
-      <c r="K26" s="99" t="s">
+      <c r="I26" s="108"/>
+      <c r="J26" s="108"/>
+      <c r="K26" s="76" t="s">
         <v>132</v>
       </c>
       <c r="L26" s="16" t="s">
@@ -11390,16 +11390,16 @@
       <c r="E27">
         <v>3</v>
       </c>
-      <c r="F27" s="94" t="s">
+      <c r="F27" s="117" t="s">
         <v>134</v>
       </c>
-      <c r="G27" s="97"/>
-      <c r="H27" s="68" t="s">
+      <c r="G27" s="118"/>
+      <c r="H27" s="108" t="s">
         <v>137</v>
       </c>
-      <c r="I27" s="68"/>
-      <c r="J27" s="68"/>
-      <c r="K27" s="99" t="s">
+      <c r="I27" s="108"/>
+      <c r="J27" s="108"/>
+      <c r="K27" s="76" t="s">
         <v>132</v>
       </c>
       <c r="L27" s="16" t="s">
@@ -11412,16 +11412,16 @@
       <c r="E28">
         <v>4</v>
       </c>
-      <c r="F28" s="94" t="s">
+      <c r="F28" s="117" t="s">
         <v>96</v>
       </c>
-      <c r="G28" s="97"/>
-      <c r="H28" s="68" t="s">
+      <c r="G28" s="118"/>
+      <c r="H28" s="108" t="s">
         <v>137</v>
       </c>
-      <c r="I28" s="68"/>
-      <c r="J28" s="68"/>
-      <c r="K28" s="99" t="s">
+      <c r="I28" s="108"/>
+      <c r="J28" s="108"/>
+      <c r="K28" s="76" t="s">
         <v>132</v>
       </c>
       <c r="L28" s="16" t="s">
@@ -11434,16 +11434,16 @@
       <c r="E29">
         <v>5</v>
       </c>
-      <c r="F29" s="94" t="s">
+      <c r="F29" s="117" t="s">
         <v>135</v>
       </c>
-      <c r="G29" s="97"/>
-      <c r="H29" s="68" t="s">
+      <c r="G29" s="118"/>
+      <c r="H29" s="108" t="s">
         <v>138</v>
       </c>
-      <c r="I29" s="68"/>
-      <c r="J29" s="68"/>
-      <c r="K29" s="99" t="s">
+      <c r="I29" s="108"/>
+      <c r="J29" s="108"/>
+      <c r="K29" s="76" t="s">
         <v>132</v>
       </c>
       <c r="L29" s="16" t="s">
@@ -11456,16 +11456,16 @@
       <c r="E30">
         <v>6</v>
       </c>
-      <c r="F30" s="94" t="s">
+      <c r="F30" s="117" t="s">
         <v>136</v>
       </c>
-      <c r="G30" s="97"/>
-      <c r="H30" s="68" t="s">
+      <c r="G30" s="118"/>
+      <c r="H30" s="108" t="s">
         <v>46</v>
       </c>
-      <c r="I30" s="68"/>
-      <c r="J30" s="68"/>
-      <c r="K30" s="99" t="s">
+      <c r="I30" s="108"/>
+      <c r="J30" s="108"/>
+      <c r="K30" s="76" t="s">
         <v>132</v>
       </c>
       <c r="L30" s="16" t="s">
@@ -11481,21 +11481,21 @@
     <mergeCell ref="J15:K16"/>
     <mergeCell ref="E12:F12"/>
     <mergeCell ref="H25:J25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F30:G30"/>
     <mergeCell ref="H26:J26"/>
     <mergeCell ref="H27:J27"/>
     <mergeCell ref="H28:J28"/>
     <mergeCell ref="H29:J29"/>
     <mergeCell ref="H30:J30"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="E18:F18"/>
     <mergeCell ref="P20:Q20"/>
     <mergeCell ref="F24:G24"/>
     <mergeCell ref="H24:J24"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="F27:G27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>